<commit_message>
Fix the csv missing fields for Aquitanian mapping file
</commit_message>
<xml_diff>
--- a/resources/4_mei_encoding/Iberian_aquitanian_notation/AQUITANIANnotation-NClevel.xlsx
+++ b/resources/4_mei_encoding/Iberian_aquitanian_notation/AQUITANIANnotation-NClevel.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2" conformance="strict">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10119"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10315"/>
   <workbookPr dateCompatibility="0" defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mthomae/Downloads/OMR_Portuguese_Sources/resources/4_mei_encoding/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mthomae/Downloads/OMR_Portuguese_Sources/resources/4_mei_encoding/Iberian_aquitanian_notation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{5FBED1BC-E3BA-094B-96DC-A9405E123B0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{DDD96722-01C9-8B4A-8EC5-435AEA7AC7C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1860" yWindow="500" windowWidth="46740" windowHeight="17440" xr2:uid="{0394C6CE-5AF9-CF4B-B63B-6BC72F9E9ED6}"/>
   </bookViews>
@@ -167,7 +167,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="106" uniqueCount="85">
+<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="132" uniqueCount="86">
   <si>
     <t>imagePath</t>
   </si>
@@ -464,6 +464,9 @@
         &lt;liquescent/&gt;
     &lt;/nc&gt;
 &lt;/neume&gt;</t>
+  </si>
+  <si>
+    <t>[]</t>
   </si>
 </sst>
 </file>
@@ -1453,8 +1456,8 @@
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A001BD3-14A6-E347-AC0D-A7B160A0B128}">
   <dimension ref="A1:K15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView tabSelected="1" topLeftCell="E11" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+      <selection activeCell="I15" sqref="I15:J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1532,6 +1535,12 @@
       <c r="H2" t="s">
         <v>13</v>
       </c>
+      <c r="I2" t="s">
+        <v>85</v>
+      </c>
+      <c r="J2" t="s">
+        <v>85</v>
+      </c>
       <c r="K2" t="s">
         <v>32</v>
       </c>
@@ -1561,6 +1570,12 @@
       <c r="H3" s="1" t="s">
         <v>16</v>
       </c>
+      <c r="I3" t="s">
+        <v>85</v>
+      </c>
+      <c r="J3" t="s">
+        <v>85</v>
+      </c>
       <c r="K3" t="s">
         <v>32</v>
       </c>
@@ -1590,6 +1605,12 @@
       <c r="H4" s="1" t="s">
         <v>17</v>
       </c>
+      <c r="I4" t="s">
+        <v>85</v>
+      </c>
+      <c r="J4" t="s">
+        <v>85</v>
+      </c>
       <c r="K4" t="s">
         <v>32</v>
       </c>
@@ -1619,6 +1640,12 @@
       <c r="H5" s="1" t="s">
         <v>20</v>
       </c>
+      <c r="I5" t="s">
+        <v>85</v>
+      </c>
+      <c r="J5" t="s">
+        <v>85</v>
+      </c>
       <c r="K5" t="s">
         <v>32</v>
       </c>
@@ -1648,6 +1675,12 @@
       <c r="H6" s="1" t="s">
         <v>78</v>
       </c>
+      <c r="I6" t="s">
+        <v>85</v>
+      </c>
+      <c r="J6" t="s">
+        <v>85</v>
+      </c>
       <c r="K6" t="s">
         <v>32</v>
       </c>
@@ -1677,6 +1710,12 @@
       <c r="H7" s="1" t="s">
         <v>84</v>
       </c>
+      <c r="I7" t="s">
+        <v>85</v>
+      </c>
+      <c r="J7" t="s">
+        <v>85</v>
+      </c>
       <c r="K7" t="s">
         <v>32</v>
       </c>
@@ -1706,6 +1745,12 @@
       <c r="H8" s="1" t="s">
         <v>25</v>
       </c>
+      <c r="I8" t="s">
+        <v>85</v>
+      </c>
+      <c r="J8" t="s">
+        <v>85</v>
+      </c>
       <c r="K8" t="s">
         <v>32</v>
       </c>
@@ -1735,6 +1780,12 @@
       <c r="H9" s="1" t="s">
         <v>28</v>
       </c>
+      <c r="I9" t="s">
+        <v>85</v>
+      </c>
+      <c r="J9" t="s">
+        <v>85</v>
+      </c>
       <c r="K9" t="s">
         <v>32</v>
       </c>
@@ -1764,6 +1815,12 @@
       <c r="H10" s="1" t="s">
         <v>79</v>
       </c>
+      <c r="I10" t="s">
+        <v>85</v>
+      </c>
+      <c r="J10" t="s">
+        <v>85</v>
+      </c>
       <c r="K10" t="s">
         <v>32</v>
       </c>
@@ -1793,6 +1850,12 @@
       <c r="H11" s="1" t="s">
         <v>80</v>
       </c>
+      <c r="I11" t="s">
+        <v>85</v>
+      </c>
+      <c r="J11" t="s">
+        <v>85</v>
+      </c>
       <c r="K11" t="s">
         <v>32</v>
       </c>
@@ -1822,6 +1885,12 @@
       <c r="H12" s="1" t="s">
         <v>81</v>
       </c>
+      <c r="I12" t="s">
+        <v>85</v>
+      </c>
+      <c r="J12" t="s">
+        <v>85</v>
+      </c>
       <c r="K12" t="s">
         <v>32</v>
       </c>
@@ -1851,6 +1920,12 @@
       <c r="H13" s="1" t="s">
         <v>82</v>
       </c>
+      <c r="I13" t="s">
+        <v>85</v>
+      </c>
+      <c r="J13" t="s">
+        <v>85</v>
+      </c>
       <c r="K13" t="s">
         <v>32</v>
       </c>
@@ -1879,6 +1954,12 @@
       </c>
       <c r="H14" s="1" t="s">
         <v>83</v>
+      </c>
+      <c r="I14" t="s">
+        <v>85</v>
+      </c>
+      <c r="J14" t="s">
+        <v>85</v>
       </c>
       <c r="K14" t="s">
         <v>32</v>

</xml_diff>

<commit_message>
Change virga to @tilt=n
</commit_message>
<xml_diff>
--- a/resources/4_mei_encoding/Iberian_aquitanian_notation/AQUITANIANnotation-NClevel.xlsx
+++ b/resources/4_mei_encoding/Iberian_aquitanian_notation/AQUITANIANnotation-NClevel.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2" conformance="strict">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10402"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10608"/>
   <workbookPr dateCompatibility="0" defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mthomae/Downloads/OMR_Portuguese_Sources/resources/4_mei_encoding/Iberian_aquitanian_notation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{168E57E6-6236-EC47-9F24-D03D1BCFC24A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{D20C052B-8D8D-C44D-AC59-0C5E63D4864C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22340" yWindow="7480" windowWidth="27440" windowHeight="17440" xr2:uid="{0394C6CE-5AF9-CF4B-B63B-6BC72F9E9ED6}"/>
+    <workbookView xWindow="3460" yWindow="3700" windowWidth="44360" windowHeight="22960" xr2:uid="{0394C6CE-5AF9-CF4B-B63B-6BC72F9E9ED6}"/>
   </bookViews>
   <sheets>
     <sheet name="AQUITANIANnotation-NClevel" sheetId="1" r:id="rId1"/>
@@ -253,11 +253,6 @@
     <t>neume.virga</t>
   </si>
   <si>
-    <t>&lt;neume&gt;
-    &lt;nc tilt="ne"/&gt;
-&lt;/neume&gt;</t>
-  </si>
-  <si>
     <t>Epiphonus</t>
   </si>
   <si>
@@ -536,12 +531,37 @@
   <si>
     <t>46v</t>
   </si>
+  <si>
+    <r>
+      <t>&lt;neume&gt;
+    &lt;nc tilt=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Aptos Narrow (Body)"/>
+      </rPr>
+      <t>"ne"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>/&gt;
+&lt;/neume&gt;</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -681,6 +701,11 @@
       <color theme="1"/>
       <name val="Helvetica Neue"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Aptos Narrow (Body)"/>
     </font>
   </fonts>
   <fills count="33">
@@ -1541,8 +1566,8 @@
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A001BD3-14A6-E347-AC0D-A7B160A0B128}">
   <dimension ref="A1:K16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1597,7 +1622,7 @@
     </row>
     <row r="2" spans="1:11" ht="82" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B2" t="e" vm="1">
         <v>#VALUE!</v>
@@ -1606,10 +1631,10 @@
         <v>11</v>
       </c>
       <c r="D2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E2" t="s">
         <v>30</v>
-      </c>
-      <c r="E2" t="s">
-        <v>31</v>
       </c>
       <c r="F2" t="s">
         <v>12</v>
@@ -1621,18 +1646,18 @@
         <v>13</v>
       </c>
       <c r="I2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="J2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="K2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="82" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B3" t="e" vm="2">
         <v>#VALUE!</v>
@@ -1641,10 +1666,10 @@
         <v>14</v>
       </c>
       <c r="D3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E3" t="s">
         <v>34</v>
-      </c>
-      <c r="E3" t="s">
-        <v>35</v>
       </c>
       <c r="F3" t="s">
         <v>15</v>
@@ -1656,33 +1681,33 @@
         <v>16</v>
       </c>
       <c r="I3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="J3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="K3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="82" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B4" t="e" vm="3">
         <v>#VALUE!</v>
       </c>
       <c r="C4" t="s">
+        <v>36</v>
+      </c>
+      <c r="D4" t="s">
         <v>37</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>38</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>39</v>
-      </c>
-      <c r="F4" t="s">
-        <v>40</v>
       </c>
       <c r="G4">
         <v>1</v>
@@ -1691,18 +1716,18 @@
         <v>17</v>
       </c>
       <c r="I4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="J4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="K4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="82" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B5" t="e" vm="4">
         <v>#VALUE!</v>
@@ -1711,10 +1736,10 @@
         <v>18</v>
       </c>
       <c r="D5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F5" t="s">
         <v>19</v>
@@ -1723,401 +1748,401 @@
         <v>1</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>20</v>
+        <v>98</v>
       </c>
       <c r="I5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="J5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="K5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="82" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B6" t="e" vm="5">
         <v>#VALUE!</v>
       </c>
       <c r="C6" t="s">
+        <v>43</v>
+      </c>
+      <c r="D6" t="s">
+        <v>33</v>
+      </c>
+      <c r="E6" t="s">
         <v>44</v>
       </c>
-      <c r="D6" t="s">
-        <v>34</v>
-      </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
         <v>45</v>
-      </c>
-      <c r="F6" t="s">
-        <v>46</v>
       </c>
       <c r="G6">
         <v>1</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="I6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="J6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="K6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="82" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B7" t="e" vm="6">
         <v>#VALUE!</v>
       </c>
       <c r="C7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7" t="s">
+        <v>47</v>
+      </c>
+      <c r="E7" t="s">
+        <v>48</v>
+      </c>
+      <c r="F7" t="s">
         <v>21</v>
-      </c>
-      <c r="D7" t="s">
-        <v>48</v>
-      </c>
-      <c r="E7" t="s">
-        <v>49</v>
-      </c>
-      <c r="F7" t="s">
-        <v>22</v>
       </c>
       <c r="G7">
         <v>1</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="I7" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="J7" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="K7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="82" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B8" t="e" vm="7">
         <v>#VALUE!</v>
       </c>
       <c r="C8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8" t="s">
+        <v>37</v>
+      </c>
+      <c r="E8" t="s">
+        <v>50</v>
+      </c>
+      <c r="F8" t="s">
         <v>23</v>
-      </c>
-      <c r="D8" t="s">
-        <v>38</v>
-      </c>
-      <c r="E8" t="s">
-        <v>51</v>
-      </c>
-      <c r="F8" t="s">
-        <v>24</v>
       </c>
       <c r="G8">
         <v>1</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="J8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="K8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="82" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B9" t="e" vm="8">
         <v>#VALUE!</v>
       </c>
       <c r="C9" t="s">
+        <v>25</v>
+      </c>
+      <c r="D9" t="s">
+        <v>29</v>
+      </c>
+      <c r="E9" t="s">
+        <v>52</v>
+      </c>
+      <c r="F9" t="s">
         <v>26</v>
-      </c>
-      <c r="D9" t="s">
-        <v>30</v>
-      </c>
-      <c r="E9" t="s">
-        <v>53</v>
-      </c>
-      <c r="F9" t="s">
-        <v>27</v>
       </c>
       <c r="G9">
         <v>1</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I9" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="J9" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="K9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="82" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B10" t="e" vm="9">
         <v>#VALUE!</v>
       </c>
       <c r="C10" t="s">
+        <v>54</v>
+      </c>
+      <c r="D10" t="s">
         <v>55</v>
       </c>
-      <c r="D10" t="s">
+      <c r="E10" t="s">
         <v>56</v>
       </c>
-      <c r="E10" t="s">
+      <c r="F10" t="s">
         <v>57</v>
       </c>
-      <c r="F10" t="s">
+      <c r="G10" t="s">
         <v>58</v>
       </c>
-      <c r="G10" t="s">
-        <v>59</v>
-      </c>
       <c r="H10" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I10" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="J10" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="K10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="82" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B11" t="e" vm="10">
         <v>#VALUE!</v>
       </c>
       <c r="C11" t="s">
+        <v>60</v>
+      </c>
+      <c r="D11" t="s">
+        <v>33</v>
+      </c>
+      <c r="E11" t="s">
         <v>61</v>
       </c>
-      <c r="D11" t="s">
-        <v>34</v>
-      </c>
-      <c r="E11" t="s">
+      <c r="F11" t="s">
         <v>62</v>
       </c>
-      <c r="F11" t="s">
-        <v>63</v>
-      </c>
       <c r="G11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I11" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="J11" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="K11" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="82" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B12" t="e" vm="11">
         <v>#VALUE!</v>
       </c>
       <c r="C12" t="s">
+        <v>64</v>
+      </c>
+      <c r="D12" t="s">
         <v>65</v>
       </c>
-      <c r="D12" t="s">
+      <c r="E12" t="s">
         <v>66</v>
       </c>
-      <c r="E12" t="s">
+      <c r="F12" t="s">
         <v>67</v>
       </c>
-      <c r="F12" t="s">
-        <v>68</v>
-      </c>
       <c r="G12" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I12" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="J12" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="K12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="13" spans="1:11" ht="82" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B13" t="e" vm="12">
         <v>#VALUE!</v>
       </c>
       <c r="C13" t="s">
+        <v>69</v>
+      </c>
+      <c r="D13" t="s">
         <v>70</v>
       </c>
-      <c r="D13" t="s">
+      <c r="E13" t="s">
         <v>71</v>
       </c>
-      <c r="E13" t="s">
+      <c r="F13" t="s">
         <v>72</v>
       </c>
-      <c r="F13" t="s">
-        <v>73</v>
-      </c>
       <c r="G13" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="I13" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="J13" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="K13" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="14" spans="1:11" ht="82" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B14" t="e" vm="13">
         <v>#VALUE!</v>
       </c>
       <c r="C14" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D14" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E14" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F14" t="s">
+        <v>88</v>
+      </c>
+      <c r="G14" t="s">
+        <v>58</v>
+      </c>
+      <c r="H14" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="G14" t="s">
-        <v>59</v>
-      </c>
-      <c r="H14" s="1" t="s">
-        <v>90</v>
-      </c>
       <c r="I14" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="J14" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="K14" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="15" spans="1:11" ht="82" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B15" t="e" vm="14">
         <v>#VALUE!</v>
       </c>
       <c r="C15" t="s">
+        <v>74</v>
+      </c>
+      <c r="D15" t="s">
+        <v>29</v>
+      </c>
+      <c r="E15" t="s">
         <v>75</v>
       </c>
-      <c r="D15" t="s">
-        <v>30</v>
-      </c>
-      <c r="E15" t="s">
+      <c r="F15" t="s">
         <v>76</v>
-      </c>
-      <c r="F15" t="s">
-        <v>77</v>
       </c>
       <c r="G15">
         <v>1</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="I15" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="J15" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="K15" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="102" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B16" s="2" t="e" vm="15">
         <v>#VALUE!</v>
       </c>
       <c r="C16" t="s">
+        <v>92</v>
+      </c>
+      <c r="D16" t="s">
+        <v>97</v>
+      </c>
+      <c r="E16" t="s">
         <v>93</v>
       </c>
-      <c r="D16" t="s">
-        <v>98</v>
-      </c>
-      <c r="E16" t="s">
-        <v>94</v>
-      </c>
       <c r="F16" t="s">
+        <v>86</v>
+      </c>
+      <c r="G16" t="s">
+        <v>91</v>
+      </c>
+      <c r="H16" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="G16" t="s">
-        <v>92</v>
-      </c>
-      <c r="H16" s="1" t="s">
-        <v>88</v>
-      </c>
       <c r="I16" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="J16" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="K16" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add possiblity of encoding just 'end of torculus'
</commit_message>
<xml_diff>
--- a/resources/4_mei_encoding/Iberian_aquitanian_notation/AQUITANIANnotation-NClevel.xlsx
+++ b/resources/4_mei_encoding/Iberian_aquitanian_notation/AQUITANIANnotation-NClevel.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2" conformance="strict">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10608"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
   <workbookPr dateCompatibility="0" defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mthomae/Downloads/OMR_Portuguese_Sources/resources/4_mei_encoding/Iberian_aquitanian_notation/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mthomae/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{D20C052B-8D8D-C44D-AC59-0C5E63D4864C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{1758366C-9BC8-7F42-B942-498513B657CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3460" yWindow="3700" windowWidth="44360" windowHeight="22960" xr2:uid="{0394C6CE-5AF9-CF4B-B63B-6BC72F9E9ED6}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="35100" windowHeight="26160" xr2:uid="{0394C6CE-5AF9-CF4B-B63B-6BC72F9E9ED6}"/>
   </bookViews>
   <sheets>
     <sheet name="AQUITANIANnotation-NClevel" sheetId="1" r:id="rId1"/>
@@ -708,7 +708,7 @@
       <name val="Aptos Narrow (Body)"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -888,8 +888,20 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.89999084444715716"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <start/>
       <end/>
@@ -1004,6 +1016,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <start style="thin">
+        <color indexed="64"/>
+      </start>
+      <end style="thin">
+        <color indexed="64"/>
+      </end>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1049,12 +1076,21 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1566,8 +1602,8 @@
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A001BD3-14A6-E347-AC0D-A7B160A0B128}">
   <dimension ref="A1:K16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="Q13" sqref="Q13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1586,562 +1622,562 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="82" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+      <c r="A2" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B2" t="e" vm="1">
+      <c r="B2" s="1" t="e" vm="1">
         <v>#VALUE!</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="G2">
+      <c r="G2" s="1">
         <v>1</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="I2" t="s">
-        <v>84</v>
-      </c>
-      <c r="J2" t="s">
-        <v>84</v>
-      </c>
-      <c r="K2" t="s">
+      <c r="I2" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="K2" s="1" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="82" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+      <c r="A3" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B3" t="e" vm="2">
+      <c r="B3" s="1" t="e" vm="2">
         <v>#VALUE!</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G3">
+      <c r="G3" s="1">
         <v>1</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="H3" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="I3" t="s">
-        <v>84</v>
-      </c>
-      <c r="J3" t="s">
-        <v>84</v>
-      </c>
-      <c r="K3" t="s">
+      <c r="I3" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="K3" s="1" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="82" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+      <c r="A4" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B4" t="e" vm="3">
+      <c r="B4" s="1" t="e" vm="3">
         <v>#VALUE!</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F4" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="G4">
+      <c r="G4" s="1">
         <v>1</v>
       </c>
-      <c r="H4" s="1" t="s">
+      <c r="H4" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="I4" t="s">
-        <v>84</v>
-      </c>
-      <c r="J4" t="s">
-        <v>84</v>
-      </c>
-      <c r="K4" t="s">
+      <c r="I4" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="K4" s="1" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="82" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+      <c r="A5" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B5" t="e" vm="4">
+      <c r="B5" s="1" t="e" vm="4">
         <v>#VALUE!</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="F5" t="s">
+      <c r="F5" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="G5">
+      <c r="G5" s="1">
         <v>1</v>
       </c>
-      <c r="H5" s="1" t="s">
+      <c r="H5" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="I5" t="s">
-        <v>84</v>
-      </c>
-      <c r="J5" t="s">
-        <v>84</v>
-      </c>
-      <c r="K5" t="s">
+      <c r="I5" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="K5" s="1" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="82" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+      <c r="A6" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B6" t="e" vm="5">
+      <c r="B6" s="1" t="e" vm="5">
         <v>#VALUE!</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="F6" t="s">
+      <c r="F6" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="G6">
+      <c r="G6" s="1">
         <v>1</v>
       </c>
-      <c r="H6" s="1" t="s">
+      <c r="H6" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="I6" t="s">
-        <v>84</v>
-      </c>
-      <c r="J6" t="s">
-        <v>84</v>
-      </c>
-      <c r="K6" t="s">
+      <c r="I6" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="K6" s="1" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="82" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+      <c r="A7" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B7" t="e" vm="6">
+      <c r="B7" s="1" t="e" vm="6">
         <v>#VALUE!</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E7" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="F7" t="s">
+      <c r="F7" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="G7">
+      <c r="G7" s="1">
         <v>1</v>
       </c>
-      <c r="H7" s="1" t="s">
+      <c r="H7" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="I7" t="s">
-        <v>84</v>
-      </c>
-      <c r="J7" t="s">
-        <v>84</v>
-      </c>
-      <c r="K7" t="s">
+      <c r="I7" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="K7" s="1" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="82" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
+      <c r="A8" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B8" t="e" vm="7">
+      <c r="B8" s="1" t="e" vm="7">
         <v>#VALUE!</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E8" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="F8" t="s">
+      <c r="F8" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="G8">
+      <c r="G8" s="1">
         <v>1</v>
       </c>
-      <c r="H8" s="1" t="s">
+      <c r="H8" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="I8" t="s">
-        <v>84</v>
-      </c>
-      <c r="J8" t="s">
-        <v>84</v>
-      </c>
-      <c r="K8" t="s">
+      <c r="I8" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="K8" s="1" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="82" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
+      <c r="A9" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B9" t="e" vm="8">
+      <c r="B9" s="1" t="e" vm="8">
         <v>#VALUE!</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E9" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="F9" t="s">
+      <c r="F9" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="G9">
+      <c r="G9" s="1">
         <v>1</v>
       </c>
-      <c r="H9" s="1" t="s">
+      <c r="H9" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="I9" t="s">
-        <v>84</v>
-      </c>
-      <c r="J9" t="s">
-        <v>84</v>
-      </c>
-      <c r="K9" t="s">
+      <c r="I9" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="K9" s="1" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="82" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
+      <c r="A10" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="B10" t="e" vm="9">
+      <c r="B10" s="4" t="e" vm="9">
         <v>#VALUE!</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E10" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="F10" t="s">
+      <c r="F10" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="G10" t="s">
+      <c r="G10" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="H10" s="1" t="s">
+      <c r="H10" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="I10" t="s">
-        <v>84</v>
-      </c>
-      <c r="J10" t="s">
-        <v>84</v>
-      </c>
-      <c r="K10" t="s">
+      <c r="I10" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="J10" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="K10" s="4" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="82" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
+      <c r="A11" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="B11" t="e" vm="10">
+      <c r="B11" s="6" t="e" vm="10">
         <v>#VALUE!</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D11" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E11" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="F11" t="s">
+      <c r="F11" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="G11" t="s">
+      <c r="G11" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="H11" s="1" t="s">
+      <c r="H11" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="I11" t="s">
-        <v>84</v>
-      </c>
-      <c r="J11" t="s">
-        <v>84</v>
-      </c>
-      <c r="K11" t="s">
+      <c r="I11" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="J11" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="K11" s="6" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="82" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
+      <c r="A12" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="B12" t="e" vm="11">
+      <c r="B12" s="4" t="e" vm="11">
         <v>#VALUE!</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D12" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E12" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="F12" t="s">
+      <c r="F12" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="G12" t="s">
+      <c r="G12" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="H12" s="1" t="s">
+      <c r="H12" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="I12" t="s">
-        <v>84</v>
-      </c>
-      <c r="J12" t="s">
-        <v>84</v>
-      </c>
-      <c r="K12" t="s">
+      <c r="I12" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="J12" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="K12" s="4" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="13" spans="1:11" ht="82" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
+      <c r="A13" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="B13" t="e" vm="12">
+      <c r="B13" s="6" t="e" vm="12">
         <v>#VALUE!</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D13" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="E13" t="s">
+      <c r="E13" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="F13" t="s">
+      <c r="F13" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="G13" t="s">
+      <c r="G13" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="H13" s="1" t="s">
+      <c r="H13" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="I13" t="s">
-        <v>84</v>
-      </c>
-      <c r="J13" t="s">
-        <v>84</v>
-      </c>
-      <c r="K13" t="s">
+      <c r="I13" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="J13" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="K13" s="6" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="14" spans="1:11" ht="82" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
+      <c r="A14" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="B14" t="e" vm="13">
+      <c r="B14" s="4" t="e" vm="13">
         <v>#VALUE!</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D14" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="E14" t="s">
+      <c r="E14" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="F14" t="s">
+      <c r="F14" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="G14" t="s">
+      <c r="G14" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="H14" s="1" t="s">
+      <c r="H14" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="I14" t="s">
-        <v>84</v>
-      </c>
-      <c r="J14" t="s">
-        <v>84</v>
-      </c>
-      <c r="K14" t="s">
+      <c r="I14" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="J14" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="K14" s="4" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="15" spans="1:11" ht="82" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
+      <c r="A15" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="B15" t="e" vm="14">
+      <c r="B15" s="1" t="e" vm="14">
         <v>#VALUE!</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D15" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="E15" t="s">
+      <c r="E15" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="F15" t="s">
+      <c r="F15" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="G15">
+      <c r="G15" s="1">
         <v>1</v>
       </c>
-      <c r="H15" s="1" t="s">
+      <c r="H15" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="I15" t="s">
-        <v>84</v>
-      </c>
-      <c r="J15" t="s">
-        <v>84</v>
-      </c>
-      <c r="K15" t="s">
+      <c r="I15" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="J15" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="K15" s="1" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="102" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
+      <c r="A16" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="B16" s="2" t="e" vm="15">
+      <c r="B16" s="3" t="e" vm="15">
         <v>#VALUE!</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C16" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D16" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="E16" t="s">
+      <c r="E16" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="F16" t="s">
+      <c r="F16" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="G16" t="s">
+      <c r="G16" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="H16" s="1" t="s">
+      <c r="H16" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="I16" t="s">
-        <v>84</v>
-      </c>
-      <c r="J16" t="s">
-        <v>84</v>
-      </c>
-      <c r="K16" t="s">
+      <c r="I16" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="J16" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="K16" s="1" t="s">
         <v>31</v>
       </c>
     </row>

</xml_diff>